<commit_message>
CIERRE 8 JUL 22
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/VENTAS MAYO CENTRAL 2022.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO   2 0 2 2/CENTRAL #05  MAYO  2022/VENTAS MAYO CENTRAL 2022.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="11220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="11220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="REMISIONES MAYO 2022" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="   C L I E N T  E S       " sheetId="2" r:id="rId2"/>
+    <sheet name="ZAVALETA  " sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -960,10 +960,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
   <dimension ref="A1:J295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C301" sqref="C301"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10391,10 +10394,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="B3:K294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19757,10 +19763,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.499984740745262"/>
+  </sheetPr>
   <dimension ref="B2:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20672,14 +20681,18 @@
     </row>
     <row r="39" spans="2:9" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C39" s="27"/>
-      <c r="D39" s="26"/>
+      <c r="D39" s="26">
+        <v>0</v>
+      </c>
       <c r="E39" s="27"/>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
     </row>
     <row r="40" spans="2:9" s="20" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C40" s="27"/>
-      <c r="D40" s="26"/>
+      <c r="D40" s="26">
+        <v>0</v>
+      </c>
       <c r="E40" s="27"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>

</xml_diff>